<commit_message>
getting spring event sizes
but still have work to do, because there is something strange going on
</commit_message>
<xml_diff>
--- a/Hydrophones/Results/noise_corrected/calculations/event1_results.xlsx
+++ b/Hydrophones/Results/noise_corrected/calculations/event1_results.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\Hydrophones\Results\noise_corrected\calculations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\GitHub\La_Jara\Hydrophones\Results\noise_corrected\calculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81BAB6A2-46F9-40BB-B7AF-6C73D590249D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E2227B-07BC-44A2-BBA4-AE95C68DF8A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3600" yWindow="1830" windowWidth="21600" windowHeight="11295" xr2:uid="{B7416B8A-9362-444F-89FB-DD7D5E3DE839}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B7416B8A-9362-444F-89FB-DD7D5E3DE839}"/>
   </bookViews>
   <sheets>
-    <sheet name="storm7_results" sheetId="1" r:id="rId1"/>
+    <sheet name="event 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -826,7 +826,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>storm7_results!$E$34:$E$130</c:f>
+              <c:f>'event 1'!$E$34:$E$130</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy\ h:mm</c:formatCode>
                 <c:ptCount val="97"/>
@@ -1126,7 +1126,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>storm7_results!$F$34:$F$130</c:f>
+              <c:f>'event 1'!$F$34:$F$130</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="97"/>
@@ -1730,7 +1730,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>storm7_results!$E$34:$E$130</c:f>
+              <c:f>'event 1'!$E$34:$E$130</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy\ h:mm</c:formatCode>
                 <c:ptCount val="97"/>
@@ -2030,7 +2030,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>storm7_results!$G$34:$G$130</c:f>
+              <c:f>'event 1'!$G$34:$G$130</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="97"/>
@@ -2634,7 +2634,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>storm7_results!$E$34:$E$130</c:f>
+              <c:f>'event 1'!$E$34:$E$130</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy\ h:mm</c:formatCode>
                 <c:ptCount val="97"/>
@@ -2934,7 +2934,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>storm7_results!$H$34:$H$130</c:f>
+              <c:f>'event 1'!$H$34:$H$130</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="97"/>
@@ -5532,8 +5532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C5B3EE7-9F25-49D2-9950-CA5E6E11E08F}">
   <dimension ref="A1:DN150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>